<commit_message>
Models clean up completed,
</commit_message>
<xml_diff>
--- a/public/SalesReport.xlsx
+++ b/public/SalesReport.xlsx
@@ -350,19 +350,17 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>02/12/2023</v>
+        <v>02/24/2023</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Realme x2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C2" t="str"/>
       <c r="D2">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>195000</v>
+        <v>180000</v>
       </c>
       <c r="F2" t="str">
         <v>COD</v>
@@ -373,19 +371,17 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>02/13/2023</v>
+        <v>02/24/2023</v>
       </c>
       <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Note 10</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C3" t="str"/>
       <c r="D3">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>20000</v>
+        <v>120000</v>
       </c>
       <c r="F3" t="str">
         <v>Razor Pay</v>
@@ -396,26 +392,270 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>02/14/2023</v>
+        <v>02/24/2023</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str"/>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>120000</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="G4" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str"/>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>300000</v>
+      </c>
+      <c r="F5" t="str">
+        <v>COD</v>
+      </c>
+      <c r="G5" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Oppo x3</v>
+      </c>
+      <c r="D6">
+        <v>60000</v>
+      </c>
+      <c r="E6">
+        <v>60000</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="G6" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str"/>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>60000</v>
+      </c>
+      <c r="F7" t="str">
+        <v>COD</v>
+      </c>
+      <c r="G7" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str"/>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>60000</v>
+      </c>
+      <c r="F8" t="str">
+        <v>COD</v>
+      </c>
+      <c r="G8" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str"/>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>120000</v>
+      </c>
+      <c r="F9" t="str">
+        <v>COD</v>
+      </c>
+      <c r="G9" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="str"/>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>60000</v>
+      </c>
+      <c r="F10" t="str">
+        <v>COD</v>
+      </c>
+      <c r="G10" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="C4" t="str">
-        <v>Realme x2</v>
-      </c>
-      <c r="D4">
-        <v>25000</v>
-      </c>
-      <c r="E4">
-        <v>195000</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Razor Pay</v>
-      </c>
-      <c r="G4" t="str">
-        <v>pending</v>
-      </c>
+      <c r="C11" t="str"/>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>60000</v>
+      </c>
+      <c r="F11" t="str">
+        <v>COD</v>
+      </c>
+      <c r="G11" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str"/>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>60000</v>
+      </c>
+      <c r="F12" t="str">
+        <v>COD</v>
+      </c>
+      <c r="G12" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="str"/>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>60000</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="G13" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="str"/>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>60000</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="G14" t="str">
+        <v>pending</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str"/>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="str"/>
+      <c r="G15" t="str"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>02/24/2023</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="str"/>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="str"/>
+      <c r="G16" t="str"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>